<commit_message>
add changes to naruto conversion sheet
</commit_message>
<xml_diff>
--- a/fandom_xlsx/naruto_characters.xlsx
+++ b/fandom_xlsx/naruto_characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkyz9\coding\repos\Ao3-TTS-Pronunciation\fandom_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A41CA228-0BAE-42E4-B98F-CB5B62619010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7688BD1-9ECD-4A32-BCD5-A319C93BAF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="298">
   <si>
     <t>Zaku</t>
   </si>
@@ -908,13 +908,25 @@
     <t>Roshi</t>
   </si>
   <si>
-    <t>saw-koo-rah</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Tsoo-mei</t>
   </si>
   <si>
-    <t xml:space="preserve"> ee-tah-chee</t>
+    <t>Shikamaru</t>
+  </si>
+  <si>
+    <t>shikamaarew</t>
+  </si>
+  <si>
+    <t>Choji</t>
+  </si>
+  <si>
+    <t>chouji</t>
+  </si>
+  <si>
+    <t>eetachi</t>
+  </si>
+  <si>
+    <t>sawkera</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B155"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD156"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50:F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,6 +1285,8 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,7 +1686,7 @@
         <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1792,7 +1806,7 @@
         <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2375,8 +2389,8 @@
       <c r="A138" t="s">
         <v>121</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>293</v>
+      <c r="B138" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2513,6 +2527,22 @@
       </c>
       <c r="B155" s="1" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>292</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>295</v>
+      </c>
+      <c r="B157" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>